<commit_message>
Updated list of Leppie's excluded tags
</commit_message>
<xml_diff>
--- a/SO Tag Server - explanation.xlsx
+++ b/SO Tag Server - explanation.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="19155" windowHeight="11565" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="19155" windowHeight="11565"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet4" sheetId="4" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
@@ -448,71 +448,6 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A1:A10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>382.23618274483476</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>101.47920163579211</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>596.29129917294847</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>898.3075960570086</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>883.84029663991203</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>957.54737998596147</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>15.46729941709647</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>407.60725730155343</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>862.52006591998042</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>139.30738242744223</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -810,6 +745,71 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A1:A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>382.23618274483476</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>101.47920163579211</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>596.29129917294847</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>898.3075960570086</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>883.84029663991203</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>957.54737998596147</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>15.46729941709647</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>407.60725730155343</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>862.52006591998042</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>139.30738242744223</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>

</xml_diff>